<commit_message>
chore(data): update mas sgd neer and swap point data
</commit_message>
<xml_diff>
--- a/data/SwapPoint.xlsx
+++ b/data/SwapPoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7DBBCE-6B7F-4519-AE71-85FD66957CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE03756-78DD-47D2-82DF-C67C113BD954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'2021'!$A$1:$AK$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'2022'!$A$1:$AK$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'2023'!$A$1:$AK$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2024'!$A$1:$D$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2024'!$A$1:$V$43</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="18">'2006'!$A:$A</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="17">'2007'!$A:$A</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="16">'2008'!$A:$A</definedName>
@@ -62,6 +62,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -98,7 +101,7 @@
     <t>ABS Benchmarks Administration Co Pte Ltd</t>
   </si>
   <si>
-    <t>Data Last Updated: 1 July 2024, 12pm</t>
+    <t>Data Last Updated: 5 August 2024, 12pm</t>
   </si>
 </sst>
 </file>
@@ -977,24 +980,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4183D3E5-8C12-4E43-98CB-C97F53232FE5}">
-  <dimension ref="A1:S43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Y86" sqref="Y86"/>
+      <selection pane="bottomRight" activeCell="AD28" sqref="AD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="19" width="8.7109375" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="22" width="8.7109375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1003,8 +1006,9 @@
       <c r="K1" s="6"/>
       <c r="N1" s="6"/>
       <c r="Q1" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" s="6"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1024,8 +1028,11 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="70">
         <v>45292</v>
@@ -1057,8 +1064,13 @@
       </c>
       <c r="R4" s="71"/>
       <c r="S4" s="72"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="70">
+        <v>45474</v>
+      </c>
+      <c r="U4" s="71"/>
+      <c r="V4" s="72"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -1125,12 +1137,24 @@
         <f t="shared" ref="R5:S5" si="7">O5</f>
         <v>3-mth</v>
       </c>
-      <c r="S5" s="7" t="str">
+      <c r="S5" s="12" t="str">
         <f t="shared" si="7"/>
         <v>6-mth</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" s="7" t="str">
+        <f>Q5</f>
+        <v>1-mth</v>
+      </c>
+      <c r="U5" s="7" t="str">
+        <f t="shared" ref="U5" si="8">R5</f>
+        <v>3-mth</v>
+      </c>
+      <c r="V5" s="12" t="str">
+        <f t="shared" ref="V5" si="9">S5</f>
+        <v>6-mth</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1150,8 +1174,11 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="13"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="13"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -1185,8 +1212,15 @@
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
       <c r="S7" s="19"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" s="18">
+        <v>-21.35</v>
+      </c>
+      <c r="U7" s="18">
+        <v>-58.5</v>
+      </c>
+      <c r="V7" s="19"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2</v>
       </c>
@@ -1230,8 +1264,15 @@
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
       <c r="S8" s="19"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" s="18">
+        <v>-19.750409999999999</v>
+      </c>
+      <c r="U8" s="18">
+        <v>-59.472915999999998</v>
+      </c>
+      <c r="V8" s="19"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -1277,8 +1318,17 @@
       <c r="S9" s="19">
         <v>-118.125</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" s="18">
+        <v>-19.5</v>
+      </c>
+      <c r="U9" s="18">
+        <v>-59.25</v>
+      </c>
+      <c r="V9" s="19">
+        <v>-116.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>4</v>
       </c>
@@ -1324,8 +1374,17 @@
       <c r="S10" s="19">
         <v>-118.125</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="18">
+        <v>-19.170000000000002</v>
+      </c>
+      <c r="U10" s="18">
+        <v>-57.037635999999999</v>
+      </c>
+      <c r="V10" s="19">
+        <v>-113.875496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>5</v>
       </c>
@@ -1377,8 +1436,17 @@
       <c r="S11" s="19">
         <v>-116.666664</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" s="18">
+        <v>-20.799999</v>
+      </c>
+      <c r="U11" s="18">
+        <v>-56.25</v>
+      </c>
+      <c r="V11" s="19">
+        <v>-112.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>6</v>
       </c>
@@ -1418,8 +1486,11 @@
       <c r="S12" s="19">
         <v>-116.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" s="18"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="19"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>7</v>
       </c>
@@ -1463,8 +1534,11 @@
       <c r="S13" s="19">
         <v>-116.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="19"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>8</v>
       </c>
@@ -1516,8 +1590,17 @@
       <c r="Q14" s="18"/>
       <c r="R14" s="18"/>
       <c r="S14" s="19"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" s="18">
+        <v>-20.460612999999999</v>
+      </c>
+      <c r="U14" s="18">
+        <v>-56.5</v>
+      </c>
+      <c r="V14" s="19">
+        <v>-113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>9</v>
       </c>
@@ -1563,8 +1646,17 @@
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
       <c r="S15" s="19"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" s="18">
+        <v>-20.208172000000001</v>
+      </c>
+      <c r="U15" s="18">
+        <v>-56.911594000000001</v>
+      </c>
+      <c r="V15" s="19">
+        <v>-113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>10</v>
       </c>
@@ -1604,8 +1696,17 @@
       <c r="S16" s="19">
         <v>-119</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16" s="18">
+        <v>-19.25</v>
+      </c>
+      <c r="U16" s="18">
+        <v>-58.373077000000002</v>
+      </c>
+      <c r="V16" s="19">
+        <v>-112.041664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>11</v>
       </c>
@@ -1651,8 +1752,17 @@
       <c r="S17" s="19">
         <v>-119</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17" s="18">
+        <v>-19.5</v>
+      </c>
+      <c r="U17" s="18">
+        <v>-57.193404999999998</v>
+      </c>
+      <c r="V17" s="19">
+        <v>-112.121674</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>12</v>
       </c>
@@ -1698,8 +1808,17 @@
       <c r="S18" s="19">
         <v>-119.894142</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" s="18">
+        <v>-19.848390999999999</v>
+      </c>
+      <c r="U18" s="18">
+        <v>-57.256985</v>
+      </c>
+      <c r="V18" s="19">
+        <v>-110.911766</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>13</v>
       </c>
@@ -1745,8 +1864,11 @@
       <c r="S19" s="19">
         <v>-117.04792</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="19"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>14</v>
       </c>
@@ -1792,8 +1914,11 @@
       <c r="S20" s="19">
         <v>-117.04792</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="19"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>15</v>
       </c>
@@ -1845,8 +1970,17 @@
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
       <c r="S21" s="19"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T21" s="18">
+        <v>-21.301946999999998</v>
+      </c>
+      <c r="U21" s="18">
+        <v>-57.5</v>
+      </c>
+      <c r="V21" s="19">
+        <v>-112.791664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>16</v>
       </c>
@@ -1892,8 +2026,17 @@
       <c r="Q22" s="18"/>
       <c r="R22" s="18"/>
       <c r="S22" s="19"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T22" s="18">
+        <v>-20.918248999999999</v>
+      </c>
+      <c r="U22" s="18">
+        <v>-58.700637999999998</v>
+      </c>
+      <c r="V22" s="19">
+        <v>-116.252647</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>17</v>
       </c>
@@ -1933,8 +2076,17 @@
       <c r="Q23" s="18"/>
       <c r="R23" s="18"/>
       <c r="S23" s="19"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T23" s="18">
+        <v>-20.117483</v>
+      </c>
+      <c r="U23" s="18">
+        <v>-59.535857999999998</v>
+      </c>
+      <c r="V23" s="19">
+        <v>-115.614197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>18</v>
       </c>
@@ -1980,8 +2132,17 @@
       <c r="S24" s="19">
         <v>-117.04792</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T24" s="18">
+        <v>-19.899999999999999</v>
+      </c>
+      <c r="U24" s="18">
+        <v>-58.271999000000001</v>
+      </c>
+      <c r="V24" s="19">
+        <v>-114.986717</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>19</v>
       </c>
@@ -2033,8 +2194,17 @@
       <c r="S25" s="19">
         <v>-116.199997</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T25" s="18">
+        <v>-19.899999999999999</v>
+      </c>
+      <c r="U25" s="18">
+        <v>-58.408298000000002</v>
+      </c>
+      <c r="V25" s="19">
+        <v>-114.986717</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>20</v>
       </c>
@@ -2080,8 +2250,11 @@
       <c r="S26" s="19">
         <v>-114.66027099999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="19"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>21</v>
       </c>
@@ -2127,8 +2300,11 @@
       <c r="S27" s="19">
         <v>-115.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="19"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>22</v>
       </c>
@@ -2174,8 +2350,17 @@
       <c r="Q28" s="18"/>
       <c r="R28" s="18"/>
       <c r="S28" s="19"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T28" s="18">
+        <v>-21.249212</v>
+      </c>
+      <c r="U28" s="18">
+        <v>-58.5</v>
+      </c>
+      <c r="V28" s="19">
+        <v>-115.441086</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>23</v>
       </c>
@@ -2221,8 +2406,17 @@
       <c r="Q29" s="18"/>
       <c r="R29" s="18"/>
       <c r="S29" s="19"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T29" s="18">
+        <v>-20.6</v>
+      </c>
+      <c r="U29" s="18">
+        <v>-58.366356000000003</v>
+      </c>
+      <c r="V29" s="19">
+        <v>-116.425957</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>24</v>
       </c>
@@ -2268,8 +2462,17 @@
       <c r="S30" s="19">
         <v>-115.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T30" s="18">
+        <v>-19.766622999999999</v>
+      </c>
+      <c r="U30" s="18">
+        <v>-59.457698999999998</v>
+      </c>
+      <c r="V30" s="19">
+        <v>-116.099998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>25</v>
       </c>
@@ -2315,8 +2518,17 @@
       <c r="S31" s="19">
         <v>-114</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31" s="18">
+        <v>-19.766622999999999</v>
+      </c>
+      <c r="U31" s="18">
+        <v>-58.032066</v>
+      </c>
+      <c r="V31" s="19">
+        <v>-116.099998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>26</v>
       </c>
@@ -2368,8 +2580,17 @@
       <c r="S32" s="19">
         <v>-116.13473500000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T32" s="18">
+        <v>-19.768561999999999</v>
+      </c>
+      <c r="U32" s="18">
+        <v>-58.386963000000002</v>
+      </c>
+      <c r="V32" s="19">
+        <v>-116.58197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>27</v>
       </c>
@@ -2409,8 +2630,11 @@
       <c r="S33" s="19">
         <v>-116.13473500000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+      <c r="V33" s="19"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>28</v>
       </c>
@@ -2456,8 +2680,11 @@
       <c r="S34" s="19">
         <v>-116.13473500000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
+      <c r="V34" s="19"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>29</v>
       </c>
@@ -2503,8 +2730,17 @@
       <c r="Q35" s="18"/>
       <c r="R35" s="18"/>
       <c r="S35" s="19"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35" s="18">
+        <v>-19.517555000000002</v>
+      </c>
+      <c r="U35" s="18">
+        <v>-58</v>
+      </c>
+      <c r="V35" s="19">
+        <v>-117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>30</v>
       </c>
@@ -2544,8 +2780,17 @@
       <c r="Q36" s="18"/>
       <c r="R36" s="18"/>
       <c r="S36" s="19"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36" s="18">
+        <v>-21.780161</v>
+      </c>
+      <c r="U36" s="18">
+        <v>-59</v>
+      </c>
+      <c r="V36" s="19">
+        <v>-118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>31</v>
       </c>
@@ -2579,8 +2824,17 @@
       <c r="Q37" s="18"/>
       <c r="R37" s="18"/>
       <c r="S37" s="19"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37" s="18">
+        <v>-21.1</v>
+      </c>
+      <c r="U37" s="18">
+        <v>-60.5</v>
+      </c>
+      <c r="V37" s="19">
+        <v>-118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2600,8 +2854,11 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
       <c r="S38" s="14"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="14"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B39" s="25" t="s">
         <v>5</v>
       </c>
@@ -2624,8 +2881,11 @@
       <c r="Q39" s="25"/>
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T39" s="25"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="25"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B40" s="25" t="s">
         <v>6</v>
       </c>
@@ -2648,8 +2908,11 @@
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T40" s="25"/>
+      <c r="U40" s="25"/>
+      <c r="V40" s="25"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B41" s="25"/>
       <c r="C41" s="25" t="s">
         <v>4</v>
@@ -2670,8 +2933,11 @@
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T41" s="25"/>
+      <c r="U41" s="25"/>
+      <c r="V41" s="25"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B43" s="69" t="s">
         <v>9</v>
       </c>
@@ -2680,9 +2946,11 @@
       <c r="K43" s="69"/>
       <c r="N43" s="69"/>
       <c r="Q43" s="69"/>
+      <c r="T43" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="T4:V4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
@@ -2692,11 +2960,14 @@
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" fitToWidth="2" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="42" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -5739,11 +6010,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="N39:P39"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="AI4:AK4"/>
@@ -5752,6 +6018,11 @@
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="N39:P39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -5763,7 +6034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -8840,12 +9111,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="Q4:S4"/>
@@ -8854,6 +9119,12 @@
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -8865,7 +9136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -11936,12 +12207,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="AI4:AK4"/>
@@ -11950,6 +12215,12 @@
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -11962,7 +12233,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -15069,12 +15340,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="AI4:AK4"/>
@@ -15083,6 +15348,12 @@
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -15095,7 +15366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -18195,6 +18466,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="AF4:AH4"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q4:S4"/>
@@ -18202,13 +18480,6 @@
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="AF4:AH4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -18221,7 +18492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -21328,12 +21599,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="T4:V4"/>
@@ -21342,6 +21607,12 @@
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -21354,7 +21625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -24461,6 +24732,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="AF4:AH4"/>
     <mergeCell ref="N39:P39"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:V4"/>
@@ -24468,13 +24746,6 @@
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="AF4:AH4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -24487,7 +24758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -27592,12 +27863,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="Q4:S4"/>
@@ -27606,6 +27871,12 @@
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -27618,7 +27889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -30752,7 +31023,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -33861,6 +34132,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="K4:M4"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="B4:D4"/>
@@ -33869,11 +34145,6 @@
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="AF4:AH4"/>
     <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -33886,7 +34157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AK43"/>
   <sheetViews>
@@ -37113,11 +37384,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="B4:D4"/>
@@ -37125,6 +37391,11 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="N4:P4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="W4:Y4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" fitToWidth="2" orientation="landscape" r:id="rId1"/>
@@ -37136,7 +37407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:AK43"/>
   <sheetViews>
@@ -40356,7 +40627,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:AK43"/>
   <sheetViews>
@@ -43584,7 +43855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -46839,7 +47110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -49904,7 +50175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -53097,6 +53368,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="W4:Y4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="B4:D4"/>
@@ -53104,11 +53380,6 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="N4:P4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="W4:Y4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" fitToWidth="2" orientation="landscape" r:id="rId1"/>
@@ -53120,7 +53391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -56193,7 +56464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
@@ -59264,18 +59535,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="W4:Y4"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="W4:Y4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>